<commit_message>
Updated the files for assignment 3
</commit_message>
<xml_diff>
--- a/Week3-Data-Driven-Testing/Assignment3.xlsx
+++ b/Week3-Data-Driven-Testing/Assignment3.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SeleniumProjects\Week3-Data-Driven-Testing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,9 +66,6 @@
     <t>Settings file in filesystem</t>
   </si>
   <si>
-    <t>c:\testupdate</t>
-  </si>
-  <si>
     <t>Use default maven settings</t>
   </si>
   <si>
@@ -81,6 +73,9 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>c:\test</t>
   </si>
 </sst>
 </file>
@@ -400,7 +395,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -411,7 +406,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +451,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -465,7 +460,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -476,7 +471,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -485,7 +480,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -500,7 +495,7 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -508,11 +503,11 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>